<commit_message>
add table template, widgets and example download
</commit_message>
<xml_diff>
--- a/reports/result/Сводная_таблица_по_месторождениям.xlsx
+++ b/reports/result/Сводная_таблица_по_месторождениям.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\geology_project\от Ильдара\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\for made\Pycharm-projects\Unstructured-field-data-aggregator\reports\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EAF12C-D889-4BA2-B4D7-3782837C9B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B01B2E3-27E3-47CE-86B1-9EE55DA989D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A0528918-EE30-4AB7-8895-26226FBF2744}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A0528918-EE30-4AB7-8895-26226FBF2744}"/>
   </bookViews>
   <sheets>
     <sheet name="Архангельское" sheetId="1" r:id="rId1"/>
     <sheet name="Матросовское" sheetId="8" r:id="rId2"/>
-    <sheet name="Граничное" sheetId="3" r:id="rId3"/>
-    <sheet name="Ивинское" sheetId="5" r:id="rId4"/>
+    <sheet name="Ивинское" sheetId="5" r:id="rId3"/>
+    <sheet name="Граничное" sheetId="3" r:id="rId4"/>
     <sheet name="Байданкинское" sheetId="6" r:id="rId5"/>
     <sheet name="Щербенское" sheetId="7" r:id="rId6"/>
   </sheets>
@@ -115,15 +115,9 @@
     <t>КИН, д. ед.</t>
   </si>
   <si>
-    <t>0,291 долей единиц 0,210 долей единиц 0,250 долей единиц</t>
-  </si>
-  <si>
     <t>Квыт, д. ед.</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0,464 доли ед . СВН  – 0,300 доли ед .</t>
-  </si>
-  <si>
     <t>фаменский ярус</t>
   </si>
   <si>
@@ -290,6 +284,13 @@
   </si>
   <si>
     <t>западная часть восточного закамья</t>
+  </si>
+  <si>
+    <t>0.291(III); 0.210(IV); 0.250(остальные)</t>
+  </si>
+  <si>
+    <t>0,464;
+0,300 (СВН)</t>
   </si>
 </sst>
 </file>
@@ -397,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -405,7 +406,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -417,22 +418,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -444,29 +439,42 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -484,55 +492,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>99173</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>21510</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Рисунок 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F919B10-3A8A-27CB-210D-4BC19B9D99D7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14745891" y="2321719"/>
-          <a:ext cx="15035563" cy="914479"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -832,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256C3014-DB5B-4831-B1EC-5C0F03C703CF}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,466 +809,578 @@
     <col min="8" max="8" width="12.77734375" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
     <col min="10" max="10" width="21.109375" customWidth="1"/>
-    <col min="11" max="11" width="11.21875" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
     <col min="12" max="12" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="H1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="P1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="Q1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="R1" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>50</v>
       </c>
       <c r="S1" s="6"/>
       <c r="T1" s="7"/>
     </row>
     <row r="2" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="17">
         <v>4</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="18">
         <v>29.5</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="22">
+      <c r="J2" s="16">
         <v>66.099999999999994</v>
       </c>
-      <c r="K2" s="22">
+      <c r="K2" s="16">
         <v>0.36</v>
       </c>
-      <c r="L2" s="22">
+      <c r="L2" s="16">
         <v>0.68200000000000005</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="17">
         <v>3</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="17">
         <v>0</v>
       </c>
-      <c r="O2" s="25">
+      <c r="O2" s="17">
         <v>3</v>
       </c>
-      <c r="P2" s="25">
+      <c r="P2" s="17">
         <v>0</v>
       </c>
-      <c r="Q2" s="25">
+      <c r="Q2" s="17">
         <v>0</v>
       </c>
-      <c r="R2" s="25" t="s">
+      <c r="R2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="17">
+        <v>8</v>
+      </c>
+      <c r="H3" s="18">
+        <v>18.7</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="16">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="K3" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="L3" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="M3" s="17">
+        <v>2</v>
+      </c>
+      <c r="N3" s="17">
+        <v>0</v>
+      </c>
+      <c r="O3" s="17">
+        <v>0</v>
+      </c>
+      <c r="P3" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="17">
+        <v>0</v>
+      </c>
+      <c r="R3" s="17">
+        <v>0</v>
+      </c>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="F3" s="22" t="s">
+      <c r="F4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="17">
+        <v>12</v>
+      </c>
+      <c r="H4" s="18">
+        <v>15.2</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="16">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="K4" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="L4" s="16">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="M4" s="17">
+        <v>201</v>
+      </c>
+      <c r="N4" s="17">
+        <v>190</v>
+      </c>
+      <c r="O4" s="17">
+        <v>11</v>
+      </c>
+      <c r="P4" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>1</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:20" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="17">
+        <v>9</v>
+      </c>
+      <c r="H5" s="18">
+        <v>13.5</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="16">
+        <v>79.7</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="17">
+        <v>268</v>
+      </c>
+      <c r="N5" s="17">
+        <v>201</v>
+      </c>
+      <c r="O5" s="17">
+        <v>63</v>
+      </c>
+      <c r="P5" s="17">
         <v>3</v>
       </c>
-      <c r="G3" s="23">
+      <c r="Q5" s="17">
+        <v>1</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="17">
+        <v>20</v>
+      </c>
+      <c r="H6" s="18">
+        <v>12.4</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="16">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.27</v>
+      </c>
+      <c r="L6" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="M6" s="17">
+        <v>36</v>
+      </c>
+      <c r="N6" s="17">
+        <v>34</v>
+      </c>
+      <c r="O6" s="17">
+        <v>2</v>
+      </c>
+      <c r="P6" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="17">
+        <v>0</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="17">
+        <v>7</v>
+      </c>
+      <c r="H7" s="18">
+        <v>24.1</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="16">
+        <v>86.5</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="M7" s="17">
+        <v>369</v>
+      </c>
+      <c r="N7" s="17">
+        <v>316</v>
+      </c>
+      <c r="O7" s="17">
+        <v>33</v>
+      </c>
+      <c r="P7" s="17">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="17">
+        <v>1</v>
+      </c>
+      <c r="R7" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="S7" s="4"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="24">
-        <v>18.7</v>
-      </c>
-      <c r="I3" s="22" t="s">
+      <c r="G8" s="17">
+        <v>16</v>
+      </c>
+      <c r="H8" s="18">
+        <v>20.6</v>
+      </c>
+      <c r="I8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="22">
-        <v>81.599999999999994</v>
-      </c>
-      <c r="K3" s="22">
+      <c r="J8" s="16">
+        <v>84.6</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="L8" s="16">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="M8" s="17">
+        <v>19</v>
+      </c>
+      <c r="N8" s="17">
+        <v>16</v>
+      </c>
+      <c r="O8" s="17">
+        <v>0</v>
+      </c>
+      <c r="P8" s="17">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>1</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="S8" s="4"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="17">
+        <v>13</v>
+      </c>
+      <c r="H9" s="18">
+        <v>12.6</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="16">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="K9" s="16">
         <v>0.25</v>
       </c>
-      <c r="L3" s="22">
-        <v>0.35</v>
-      </c>
-      <c r="M3" s="25">
+      <c r="L9" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="M9" s="17">
+        <v>36</v>
+      </c>
+      <c r="N9" s="17">
+        <v>27</v>
+      </c>
+      <c r="O9" s="17">
+        <v>7</v>
+      </c>
+      <c r="P9" s="17">
         <v>2</v>
       </c>
-      <c r="N3" s="25">
+      <c r="Q9" s="17">
         <v>0</v>
       </c>
-      <c r="O3" s="25">
+      <c r="R9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="F10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="17">
+        <v>1</v>
+      </c>
+      <c r="H10" s="18">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="16">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0.316</v>
+      </c>
+      <c r="L10" s="16">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="M10" s="17">
+        <v>2</v>
+      </c>
+      <c r="N10" s="17">
+        <v>1</v>
+      </c>
+      <c r="O10" s="17">
         <v>0</v>
       </c>
-      <c r="P3" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="25">
+      <c r="P10" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="17">
         <v>0</v>
       </c>
-      <c r="R3" s="25">
-        <v>0</v>
-      </c>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" s="22" t="s">
+      <c r="R10" s="17">
         <v>4</v>
       </c>
-      <c r="G4" s="23">
-        <v>12</v>
-      </c>
-      <c r="H4" s="24">
-        <v>15.9</v>
-      </c>
-      <c r="I4" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="22">
-        <v>73.400000000000006</v>
-      </c>
-      <c r="K4" s="22">
-        <v>0.25</v>
-      </c>
-      <c r="L4" s="22">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="M4" s="25">
-        <v>201</v>
-      </c>
-      <c r="N4" s="25">
-        <v>190</v>
-      </c>
-      <c r="O4" s="25">
-        <v>11</v>
-      </c>
-      <c r="P4" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="25">
-        <v>1</v>
-      </c>
-      <c r="R4" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="23">
-        <v>9</v>
-      </c>
-      <c r="H5" s="24">
-        <v>13.5</v>
-      </c>
-      <c r="I5" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="22">
-        <v>79.7</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="25">
-        <v>268</v>
-      </c>
-      <c r="N5" s="25">
-        <v>201</v>
-      </c>
-      <c r="O5" s="25">
-        <v>63</v>
-      </c>
-      <c r="P5" s="25">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="25">
-        <v>1</v>
-      </c>
-      <c r="R5" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="F6" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="23">
-        <v>20</v>
-      </c>
-      <c r="H6" s="24">
-        <v>12.4</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="22">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="K6" s="22">
-        <v>0.27</v>
-      </c>
-      <c r="L6" s="22">
-        <v>0.4</v>
-      </c>
-      <c r="M6" s="25">
-        <v>36</v>
-      </c>
-      <c r="N6" s="25">
-        <v>34</v>
-      </c>
-      <c r="O6" s="25">
-        <v>2</v>
-      </c>
-      <c r="P6" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="25">
-        <v>0</v>
-      </c>
-      <c r="R6" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="F7" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="23">
-        <v>7</v>
-      </c>
-      <c r="H7" s="24">
-        <v>24.1</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="22">
-        <v>86.5</v>
-      </c>
-      <c r="K7" s="22">
-        <v>0.46500000000000002</v>
-      </c>
-      <c r="L7" s="22">
-        <v>0.53600000000000003</v>
-      </c>
-      <c r="M7" s="25">
-        <v>369</v>
-      </c>
-      <c r="N7" s="25">
-        <v>316</v>
-      </c>
-      <c r="O7" s="25">
-        <v>33</v>
-      </c>
-      <c r="P7" s="25">
-        <v>19</v>
-      </c>
-      <c r="Q7" s="25">
-        <v>1</v>
-      </c>
-      <c r="R7" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="F8" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="23">
-        <v>16</v>
-      </c>
-      <c r="H8" s="24">
-        <v>20.6</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="22">
-        <v>84.6</v>
-      </c>
-      <c r="K8" s="22">
-        <v>0.40100000000000002</v>
-      </c>
-      <c r="L8" s="22">
-        <v>0.47299999999999998</v>
-      </c>
-      <c r="M8" s="25">
-        <v>19</v>
-      </c>
-      <c r="N8" s="25">
-        <v>16</v>
-      </c>
-      <c r="O8" s="25">
-        <v>0</v>
-      </c>
-      <c r="P8" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="25">
-        <v>1</v>
-      </c>
-      <c r="R8" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="S8" s="4"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="F9" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="23">
-        <v>13</v>
-      </c>
-      <c r="H9" s="24">
-        <v>12.6</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="22">
-        <v>68.900000000000006</v>
-      </c>
-      <c r="K9" s="22">
-        <v>0.25</v>
-      </c>
-      <c r="L9" s="22">
-        <v>0.4</v>
-      </c>
-      <c r="M9" s="25">
-        <v>36</v>
-      </c>
-      <c r="N9" s="25">
-        <v>27</v>
-      </c>
-      <c r="O9" s="25">
-        <v>7</v>
-      </c>
-      <c r="P9" s="25">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="25">
-        <v>0</v>
-      </c>
-      <c r="R9" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="S9" s="4"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="F10" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="23">
-        <v>1</v>
-      </c>
-      <c r="H10" s="24"/>
-      <c r="I10" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22">
-        <v>0.316</v>
-      </c>
-      <c r="L10" s="22">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="M10" s="25">
-        <v>2</v>
-      </c>
-      <c r="N10" s="25">
-        <v>1</v>
-      </c>
-      <c r="O10" s="25">
-        <v>0</v>
-      </c>
-      <c r="P10" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="25">
-        <v>0</v>
-      </c>
-      <c r="R10" s="25">
-        <v>4</v>
-      </c>
       <c r="S10" s="4"/>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="25"/>
+      <c r="F26" s="26"/>
+    </row>
+    <row r="27" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E27" s="25"/>
+      <c r="F27" s="26"/>
+    </row>
+    <row r="28" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="25"/>
+      <c r="F28" s="26"/>
+    </row>
+    <row r="29" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E29" s="25"/>
+      <c r="F29" s="26"/>
+    </row>
+    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E30" s="25"/>
+      <c r="F30" s="26"/>
+    </row>
+    <row r="31" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E31" s="25"/>
+      <c r="F31" s="26"/>
+    </row>
+    <row r="32" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="25"/>
+      <c r="F32" s="26"/>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E33" s="25"/>
+      <c r="F33" s="26"/>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E42" s="25"/>
+      <c r="F42" s="28"/>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E43" s="25"/>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E44" s="25"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E45" s="25"/>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E46" s="25"/>
+      <c r="F46" s="28"/>
+    </row>
+    <row r="47" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E47" s="25"/>
+      <c r="F47" s="28"/>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E48" s="25"/>
+      <c r="F48" s="28"/>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E49" s="25"/>
+      <c r="F49" s="28"/>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E50" s="25"/>
+      <c r="F50" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1324,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A410D37C-2141-43C2-AF8B-50084372A8CE}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScale="82" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,22 +1415,22 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>
@@ -1368,28 +1439,28 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4">
         <v>3</v>
@@ -1409,24 +1480,176 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C492253F-F25E-4619-A849-DA0F3433CDB4}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>13</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="4">
+        <v>23</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4">
+        <v>22</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA6B032-E062-4BBA-B6CB-393B01DCC477}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="116" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1441,16 +1664,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -1467,16 +1690,16 @@
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>12</v>
@@ -1535,163 +1758,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C492253F-F25E-4619-A849-DA0F3433CDB4}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="4">
-        <v>15</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="4">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4">
-        <v>15</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4">
         <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="4">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="4">
-        <v>23</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="4">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4">
-        <v>22</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="4">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="4">
-        <v>13</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="4">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1703,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3E4C29-4286-4F96-ACE4-C6F6B6FC4AC5}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="104" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1719,17 +1789,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>0</v>
@@ -1745,17 +1815,17 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>71</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>4</v>
@@ -1769,10 +1839,10 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1838,10 +1908,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1859,8 +1929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D071E582-4619-4083-96AC-3B220330E423}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScale="117" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1876,16 +1946,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>0</v>
@@ -1900,7 +1970,7 @@
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="3">
         <v>1969</v>
@@ -1908,8 +1978,8 @@
       <c r="C2" s="3">
         <v>2005</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>77</v>
+      <c r="D2" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -1934,10 +2004,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>